<commit_message>
edits to initial data
</commit_message>
<xml_diff>
--- a/initializationData/GliderMission.xlsx
+++ b/initializationData/GliderMission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laytonc\Documents\GitHub\gliderMetadata\initializationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB2942B-53DA-4BC6-8308-AC4429F7C472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{71DD7517-61B5-4DF9-8DB2-1A18297228CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2863,10 +2863,10 @@
   <dimension ref="A1:BP83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="AS48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="AJ48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BB65" sqref="BB65"/>
+      <selection pane="bottomRight" activeCell="AN66" sqref="AN66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13764,7 +13764,7 @@
         <v>81</v>
       </c>
       <c r="AN65" s="121" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="AO65" s="111" t="s">
         <v>218</v>

</xml_diff>